<commit_message>
Add bottom of screen back/next
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/fw_location/forms/fw_location/fw_location.xlsx
+++ b/odkx/app/config/tables/fw_location/forms/fw_location/fw_location.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kiswahili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">showFooter</t>
   </si>
   <si>
     <t xml:space="preserve">hh_id</t>
@@ -368,7 +371,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -413,7 +416,7 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
@@ -473,13 +476,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
@@ -530,7 +533,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210204001</v>
+        <v>20210221001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,6 +598,14 @@
       </c>
       <c r="H8" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -619,7 +630,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
   </cols>
@@ -634,18 +645,18 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,10 +669,10 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -682,11 +693,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.56"/>
@@ -694,16 +705,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,13 +722,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,13 +736,13 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mark geolocation questions as required
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/fw_location/forms/fw_location/fw_location.xlsx
+++ b/odkx/app/config/tables/fw_location/forms/fw_location/fw_location.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" state="visible" r:id="rId2"/>
@@ -371,7 +371,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -412,11 +412,11 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
@@ -451,7 +451,9 @@
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
@@ -478,11 +480,11 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
@@ -533,7 +535,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>20210221001</v>
+        <v>20210421001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,7 +632,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
   </cols>
@@ -697,7 +699,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.56"/>

</xml_diff>